<commit_message>
70. Gradient Descent in Action
</commit_message>
<xml_diff>
--- a/resources/mse_graph.xlsx
+++ b/resources/mse_graph.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noah/Documents/study/study_codes/udemy/machine-learning-js-stephen/machine-learning-js-stephen-git/images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noah/Documents/study/study_codes/udemy/machine-learning-js-stephen/machine-learning-js-stephen-git/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCFB29E-4358-1947-A66E-E5A8153A0606}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC328862-739A-D04C-B78A-4A66A961013D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4740" yWindow="-21580" windowWidth="29980" windowHeight="18940" xr2:uid="{4090F69A-B87C-A848-B205-CF8351D4CAAD}"/>
+    <workbookView xWindow="-1680" yWindow="-20940" windowWidth="29980" windowHeight="18940" xr2:uid="{4090F69A-B87C-A848-B205-CF8351D4CAAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Sqrt</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Guess for B</t>
   </si>
   <si>
     <t>MSE</t>
+  </si>
+  <si>
+    <t>Lot Size</t>
+  </si>
+  <si>
+    <t>House price</t>
+  </si>
+  <si>
+    <t>Learning Rate</t>
+  </si>
+  <si>
+    <t>Value of B</t>
+  </si>
+  <si>
+    <t>Initial Guess:</t>
+  </si>
+  <si>
+    <t>Slope of MSE</t>
+  </si>
+  <si>
+    <t>How Much To Adjust B</t>
   </si>
 </sst>
 </file>
@@ -46,7 +61,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -54,13 +69,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,11 +104,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2115,15 +2154,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2151,15 +2190,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>654050</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:colOff>615950</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2484,477 +2523,977 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD848182-8EBD-094B-9D79-4F6A3B7DE717}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>800</v>
       </c>
       <c r="B2" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5">
+        <f>2 * ((J2-$B$2) + (J2-$B$3) + (J2-$B$4) + (J2-$B$5) + (J2-$B$6) + (J2-$B$7)) / 6</f>
+        <v>-490</v>
+      </c>
+      <c r="L2">
+        <f>K2*$G$3</f>
+        <v>-147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>950</v>
       </c>
       <c r="B3" s="1">
         <v>230</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>0.3</v>
+      </c>
+      <c r="J3">
+        <f>J2-L2</f>
+        <v>147</v>
+      </c>
+      <c r="K3" s="5">
+        <f>2 * ((J3-$B$2) + (J3-$B$3) + (J3-$B$4) + (J3-$B$5) + (J3-$B$6) + (J3-$B$7)) / 6</f>
+        <v>-196</v>
+      </c>
+      <c r="L3">
+        <f>K3*$G$3</f>
+        <v>-58.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1040</v>
       </c>
       <c r="B4" s="1">
         <v>245</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <f t="shared" ref="J4:J27" si="0">J3-L3</f>
+        <v>205.8</v>
+      </c>
+      <c r="K4" s="5">
+        <f t="shared" ref="K4:K41" si="1">2 * ((J4-$B$2) + (J4-$B$3) + (J4-$B$4) + (J4-$B$5) + (J4-$B$6) + (J4-$B$7)) / 6</f>
+        <v>-78.399999999999977</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L41" si="2">K4*$G$3</f>
+        <v>-23.519999999999992</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1120</v>
       </c>
       <c r="B5" s="1">
         <v>274</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>229.32</v>
+      </c>
+      <c r="K5" s="5">
+        <f t="shared" si="1"/>
+        <v>-31.360000000000014</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>-9.408000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1250</v>
       </c>
       <c r="B6" s="1">
         <v>259</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>238.72800000000001</v>
+      </c>
+      <c r="K6" s="5">
+        <f t="shared" si="1"/>
+        <v>-12.543999999999983</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>-3.7631999999999945</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>1350</v>
       </c>
       <c r="B7" s="1">
         <v>262</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>242.49119999999999</v>
+      </c>
+      <c r="K7" s="5">
+        <f t="shared" si="1"/>
+        <v>-5.0176000000000158</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>-1.5052800000000046</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>243.99647999999999</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.0070400000000177</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>-0.60211200000000531</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>244.598592</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" si="1"/>
+        <v>-0.80281600000000708</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>-0.24084480000000211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>1</v>
       </c>
       <c r="B10" s="3">
-        <f t="shared" ref="B10:B49" si="0">(($A10-$B$2)^2+($A10-$B$3)^2+($A10-$B$4)^2+($A10-$B$5)^2+($A10-$B$6)^2+($A10-$B$7)^2) / 6</f>
+        <f t="shared" ref="B10:B49" si="3">(($A10-$B$2)^2+($A10-$B$3)^2+($A10-$B$4)^2+($A10-$B$5)^2+($A10-$B$6)^2+($A10-$B$7)^2) / 6</f>
         <v>60132</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>244.83943679999999</v>
+      </c>
+      <c r="K10" s="5">
+        <f t="shared" si="1"/>
+        <v>-0.32112640000002557</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>-9.6337920000007668E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <f>A10+10</f>
         <v>11</v>
       </c>
       <c r="B11" s="3">
+        <f t="shared" si="3"/>
+        <v>55352</v>
+      </c>
+      <c r="J11">
         <f t="shared" si="0"/>
-        <v>55352</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>244.93577471999998</v>
+      </c>
+      <c r="K11" s="5">
+        <f t="shared" si="1"/>
+        <v>-0.12845056000003297</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>-3.853516800000989E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <f t="shared" ref="A12:A40" si="1">A11+10</f>
+        <f t="shared" ref="A12:A40" si="4">A11+10</f>
         <v>21</v>
       </c>
       <c r="B12" s="3">
+        <f t="shared" si="3"/>
+        <v>50772</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="0"/>
-        <v>50772</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>244.97430988799999</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="1"/>
+        <v>-5.1380224000013186E-2</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>-1.5414067200003954E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="3"/>
+        <v>46392</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>244.98972395519999</v>
+      </c>
+      <c r="K13" s="5">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="B13" s="3">
+        <v>-2.0552089600016643E-2</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>-6.1656268800049929E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="3"/>
+        <v>42212</v>
+      </c>
+      <c r="J14">
         <f t="shared" si="0"/>
-        <v>46392</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+        <v>244.99588958208</v>
+      </c>
+      <c r="K14" s="5">
         <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="B14" s="3">
+        <v>-8.2208358400066572E-3</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>-2.4662507520019973E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <f t="shared" si="4"/>
+        <v>51</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="3"/>
+        <v>38232</v>
+      </c>
+      <c r="J15">
         <f t="shared" si="0"/>
-        <v>42212</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+        <v>244.998355832832</v>
+      </c>
+      <c r="K15" s="5">
         <f t="shared" si="1"/>
-        <v>51</v>
-      </c>
-      <c r="B15" s="3">
+        <v>-3.2883343359912942E-3</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>-9.8650030079738826E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <f t="shared" si="4"/>
+        <v>61</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="3"/>
+        <v>34452</v>
+      </c>
+      <c r="J16">
         <f t="shared" si="0"/>
-        <v>38232</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+        <v>244.9993423331328</v>
+      </c>
+      <c r="K16" s="5">
         <f t="shared" si="1"/>
-        <v>61</v>
-      </c>
-      <c r="B16" s="3">
+        <v>-1.3153337343965177E-3</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>-3.9460012031895532E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <f t="shared" si="4"/>
+        <v>71</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" si="3"/>
+        <v>30872</v>
+      </c>
+      <c r="J17">
         <f t="shared" si="0"/>
-        <v>34452</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+        <v>244.99973693325313</v>
+      </c>
+      <c r="K17" s="5">
         <f t="shared" si="1"/>
-        <v>71</v>
-      </c>
-      <c r="B17" s="3">
+        <v>-5.2613349373586971E-4</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>-1.578400481207609E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <f t="shared" si="4"/>
+        <v>81</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" si="3"/>
+        <v>27492</v>
+      </c>
+      <c r="J18">
         <f t="shared" si="0"/>
-        <v>30872</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+        <v>244.99989477330126</v>
+      </c>
+      <c r="K18" s="5">
         <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="B18" s="3">
+        <v>-2.1045339747161051E-4</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>-6.3136019241483149E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <f t="shared" si="4"/>
+        <v>91</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" si="3"/>
+        <v>24312</v>
+      </c>
+      <c r="J19">
         <f t="shared" si="0"/>
-        <v>27492</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+        <v>244.9999579093205</v>
+      </c>
+      <c r="K19" s="5">
         <f t="shared" si="1"/>
-        <v>91</v>
-      </c>
-      <c r="B19" s="3">
+        <v>-8.418135900001289E-5</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>-2.5254407700003866E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <f t="shared" si="4"/>
+        <v>101</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="3"/>
+        <v>21332</v>
+      </c>
+      <c r="J20">
         <f t="shared" si="0"/>
-        <v>24312</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+        <v>244.99998316372819</v>
+      </c>
+      <c r="K20" s="5">
         <f t="shared" si="1"/>
-        <v>101</v>
-      </c>
-      <c r="B20" s="3">
+        <v>-3.3672543622742523E-5</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>-1.0101763086822757E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <f t="shared" si="4"/>
+        <v>111</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" si="3"/>
+        <v>18552</v>
+      </c>
+      <c r="J21">
         <f t="shared" si="0"/>
-        <v>21332</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+        <v>244.99999326549127</v>
+      </c>
+      <c r="K21" s="5">
         <f t="shared" si="1"/>
-        <v>111</v>
-      </c>
-      <c r="B21" s="3">
+        <v>-1.3469017460465693E-5</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="2"/>
+        <v>-4.0407052381397078E-6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <f t="shared" si="4"/>
+        <v>121</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="3"/>
+        <v>15972</v>
+      </c>
+      <c r="J22">
         <f t="shared" si="0"/>
-        <v>18552</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+        <v>244.99999730619652</v>
+      </c>
+      <c r="K22" s="5">
         <f t="shared" si="1"/>
-        <v>121</v>
-      </c>
-      <c r="B22" s="3">
+        <v>-5.3876069614489097E-6</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="2"/>
+        <v>-1.6162820884346729E-6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <f t="shared" si="4"/>
+        <v>131</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" si="3"/>
+        <v>13592</v>
+      </c>
+      <c r="J23">
         <f t="shared" si="0"/>
-        <v>15972</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+        <v>244.9999989224786</v>
+      </c>
+      <c r="K23" s="5">
         <f t="shared" si="1"/>
-        <v>131</v>
-      </c>
-      <c r="B23" s="3">
+        <v>-2.1550428073169314E-6</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="2"/>
+        <v>-6.4651284219507939E-7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <f t="shared" si="4"/>
+        <v>141</v>
+      </c>
+      <c r="B24" s="3">
+        <f t="shared" si="3"/>
+        <v>11412</v>
+      </c>
+      <c r="J24" s="8">
         <f t="shared" si="0"/>
-        <v>13592</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+        <v>244.99999956899143</v>
+      </c>
+      <c r="K24" s="9">
         <f t="shared" si="1"/>
-        <v>141</v>
-      </c>
-      <c r="B24" s="3">
+        <v>-8.6201714566414012E-7</v>
+      </c>
+      <c r="L24" s="8">
+        <f t="shared" si="2"/>
+        <v>-2.5860514369924202E-7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <f t="shared" si="4"/>
+        <v>151</v>
+      </c>
+      <c r="B25" s="3">
+        <f t="shared" si="3"/>
+        <v>9432</v>
+      </c>
+      <c r="J25">
         <f t="shared" si="0"/>
-        <v>11412</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+        <v>244.99999982759658</v>
+      </c>
+      <c r="K25" s="5">
         <f t="shared" si="1"/>
-        <v>151</v>
-      </c>
-      <c r="B25" s="3">
+        <v>-3.448068355282885E-7</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="2"/>
+        <v>-1.0344205065848655E-7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <f t="shared" si="4"/>
+        <v>161</v>
+      </c>
+      <c r="B26" s="3">
+        <f t="shared" si="3"/>
+        <v>7652</v>
+      </c>
+      <c r="J26">
         <f t="shared" si="0"/>
-        <v>9432</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+        <v>244.99999993103864</v>
+      </c>
+      <c r="K26" s="5">
         <f t="shared" si="1"/>
-        <v>161</v>
-      </c>
-      <c r="B26" s="3">
+        <v>-1.3792271147394786E-7</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>-4.1376813442184356E-8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <f t="shared" si="4"/>
+        <v>171</v>
+      </c>
+      <c r="B27" s="3">
+        <f t="shared" si="3"/>
+        <v>6072</v>
+      </c>
+      <c r="J27">
         <f t="shared" si="0"/>
-        <v>7652</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+        <v>244.99999997241545</v>
+      </c>
+      <c r="K27" s="5">
         <f t="shared" si="1"/>
-        <v>171</v>
-      </c>
-      <c r="B27" s="3">
-        <f t="shared" si="0"/>
-        <v>6072</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-5.5169095958262915E-8</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>-1.6550728787478874E-8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
+        <f t="shared" si="4"/>
+        <v>181</v>
+      </c>
+      <c r="B28" s="3">
+        <f t="shared" si="3"/>
+        <v>4692</v>
+      </c>
+      <c r="J28">
+        <f>J27-L27</f>
+        <v>244.99999998896618</v>
+      </c>
+      <c r="K28" s="5">
+        <f>2 * ((J28-$B$2) + (J28-$B$3) + (J28-$B$4) + (J28-$B$5) + (J28-$B$6) + (J28-$B$7)) / 6</f>
+        <v>-2.2067638383305166E-8</v>
+      </c>
+      <c r="L28">
+        <f>K28*$G$3</f>
+        <v>-6.6202915149915494E-9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <f t="shared" si="4"/>
+        <v>191</v>
+      </c>
+      <c r="B29" s="3">
+        <f t="shared" si="3"/>
+        <v>3512</v>
+      </c>
+      <c r="J29">
+        <f t="shared" ref="J29:J33" si="5">J28-L28</f>
+        <v>244.99999999558648</v>
+      </c>
+      <c r="K29" s="5">
         <f t="shared" si="1"/>
-        <v>181</v>
-      </c>
-      <c r="B28" s="3">
-        <f t="shared" si="0"/>
-        <v>4692</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+        <v>-8.8270439846382942E-9</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>-2.6481131953914882E-9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <f t="shared" si="4"/>
+        <v>201</v>
+      </c>
+      <c r="B30" s="3">
+        <f t="shared" si="3"/>
+        <v>2532</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="5"/>
+        <v>244.99999999823459</v>
+      </c>
+      <c r="K30" s="5">
         <f t="shared" si="1"/>
-        <v>191</v>
-      </c>
-      <c r="B29" s="3">
-        <f t="shared" si="0"/>
-        <v>3512</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
+        <v>-3.5308289625390898E-9</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="2"/>
+        <v>-1.059248688761727E-9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <f t="shared" si="4"/>
+        <v>211</v>
+      </c>
+      <c r="B31" s="3">
+        <f t="shared" si="3"/>
+        <v>1752</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="5"/>
+        <v>244.99999999929383</v>
+      </c>
+      <c r="K31" s="5">
         <f t="shared" si="1"/>
-        <v>201</v>
-      </c>
-      <c r="B30" s="3">
-        <f t="shared" si="0"/>
-        <v>2532</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+        <v>-1.4123315850156359E-9</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="2"/>
+        <v>-4.2369947550469074E-10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <f t="shared" si="4"/>
+        <v>221</v>
+      </c>
+      <c r="B32" s="3">
+        <f t="shared" si="3"/>
+        <v>1172</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="5"/>
+        <v>244.99999999971755</v>
+      </c>
+      <c r="K32" s="5">
         <f t="shared" si="1"/>
-        <v>211</v>
-      </c>
-      <c r="B31" s="3">
-        <f t="shared" si="0"/>
-        <v>1752</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
+        <v>-5.6490989663871005E-10</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="2"/>
+        <v>-1.6947296899161302E-10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <f t="shared" si="4"/>
+        <v>231</v>
+      </c>
+      <c r="B33" s="3">
+        <f t="shared" si="3"/>
+        <v>792</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="5"/>
+        <v>244.99999999988702</v>
+      </c>
+      <c r="K33" s="5">
         <f t="shared" si="1"/>
-        <v>221</v>
-      </c>
-      <c r="B32" s="3">
-        <f t="shared" si="0"/>
-        <v>1172</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+        <v>-2.2595258997171186E-10</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="2"/>
+        <v>-6.7785776991513558E-11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <f t="shared" si="4"/>
+        <v>241</v>
+      </c>
+      <c r="B34" s="3">
+        <f t="shared" si="3"/>
+        <v>612</v>
+      </c>
+      <c r="J34">
+        <f>J33-L33</f>
+        <v>244.99999999995481</v>
+      </c>
+      <c r="K34" s="5">
+        <f>2 * ((J34-$B$2) + (J34-$B$3) + (J34-$B$4) + (J34-$B$5) + (J34-$B$6) + (J34-$B$7)) / 6</f>
+        <v>-9.0381035988684744E-11</v>
+      </c>
+      <c r="L34">
+        <f>K34*$G$3</f>
+        <v>-2.7114310796605423E-11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <f t="shared" si="4"/>
+        <v>251</v>
+      </c>
+      <c r="B35" s="3">
+        <f t="shared" si="3"/>
+        <v>632</v>
+      </c>
+      <c r="J35">
+        <f t="shared" ref="J35" si="6">J34-L34</f>
+        <v>244.99999999998192</v>
+      </c>
+      <c r="K35" s="5">
         <f t="shared" si="1"/>
-        <v>231</v>
-      </c>
-      <c r="B33" s="3">
-        <f t="shared" si="0"/>
-        <v>792</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
+        <v>-3.6152414395473897E-11</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="2"/>
+        <v>-1.0845724318642168E-11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <f t="shared" si="4"/>
+        <v>261</v>
+      </c>
+      <c r="B36" s="3">
+        <f t="shared" si="3"/>
+        <v>852</v>
+      </c>
+      <c r="J36">
+        <f t="shared" ref="J36:J41" si="7">J35-L35</f>
+        <v>244.99999999999278</v>
+      </c>
+      <c r="K36" s="5">
         <f t="shared" si="1"/>
-        <v>241</v>
-      </c>
-      <c r="B34" s="3">
-        <f t="shared" si="0"/>
-        <v>612</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
+        <v>-1.4438228390645236E-11</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="2"/>
+        <v>-4.3314685171935709E-12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <f t="shared" si="4"/>
+        <v>271</v>
+      </c>
+      <c r="B37" s="3">
+        <f t="shared" si="3"/>
+        <v>1272</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="7"/>
+        <v>244.9999999999971</v>
+      </c>
+      <c r="K37" s="5">
         <f t="shared" si="1"/>
-        <v>251</v>
-      </c>
-      <c r="B35" s="3">
-        <f t="shared" si="0"/>
-        <v>632</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
+        <v>-5.7980287238024175E-12</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="2"/>
+        <v>-1.7394086171407251E-12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <f t="shared" si="4"/>
+        <v>281</v>
+      </c>
+      <c r="B38" s="3">
+        <f t="shared" si="3"/>
+        <v>1892</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="7"/>
+        <v>244.99999999999883</v>
+      </c>
+      <c r="K38" s="5">
         <f t="shared" si="1"/>
-        <v>261</v>
-      </c>
-      <c r="B36" s="3">
-        <f t="shared" si="0"/>
-        <v>852</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
+        <v>-2.3305801732931286E-12</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="2"/>
+        <v>-6.9917405198793852E-13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <f t="shared" si="4"/>
+        <v>291</v>
+      </c>
+      <c r="B39" s="3">
+        <f t="shared" si="3"/>
+        <v>2712</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="7"/>
+        <v>244.99999999999955</v>
+      </c>
+      <c r="K39" s="5">
         <f t="shared" si="1"/>
-        <v>271</v>
-      </c>
-      <c r="B37" s="3">
-        <f t="shared" si="0"/>
-        <v>1272</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+        <v>-9.0949470177292824E-13</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="2"/>
+        <v>-2.7284841053187846E-13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <f t="shared" si="4"/>
+        <v>301</v>
+      </c>
+      <c r="B40" s="3">
+        <f t="shared" si="3"/>
+        <v>3732</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="7"/>
+        <v>244.99999999999983</v>
+      </c>
+      <c r="K40" s="5">
         <f t="shared" si="1"/>
-        <v>281</v>
-      </c>
-      <c r="B38" s="3">
-        <f t="shared" si="0"/>
-        <v>1892</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
+        <v>-3.4106051316484809E-13</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="2"/>
+        <v>-1.0231815394945442E-13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <f t="shared" ref="A41:A49" si="8">A40+10</f>
+        <v>311</v>
+      </c>
+      <c r="B41" s="3">
+        <f t="shared" si="3"/>
+        <v>4952</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="7"/>
+        <v>244.99999999999994</v>
+      </c>
+      <c r="K41" s="5">
         <f t="shared" si="1"/>
-        <v>291</v>
-      </c>
-      <c r="B39" s="3">
-        <f t="shared" si="0"/>
-        <v>2712</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
-        <f t="shared" si="1"/>
-        <v>301</v>
-      </c>
-      <c r="B40" s="3">
-        <f t="shared" si="0"/>
-        <v>3732</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
-        <f t="shared" ref="A41:A49" si="2">A40+10</f>
-        <v>311</v>
-      </c>
-      <c r="B41" s="3">
-        <f t="shared" si="0"/>
-        <v>4952</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1368683772161603E-13</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="2"/>
+        <v>-3.4106051316484808E-14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>321</v>
       </c>
       <c r="B42" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6372</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>331</v>
       </c>
       <c r="B43" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7992</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>341</v>
       </c>
       <c r="B44" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9812</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>351</v>
       </c>
       <c r="B45" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>11832</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>361</v>
       </c>
       <c r="B46" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>14052</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>371</v>
       </c>
       <c r="B47" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16472</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>381</v>
       </c>
       <c r="B48" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>19092</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>391</v>
       </c>
       <c r="B49" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>21912</v>
       </c>
     </row>

</xml_diff>

<commit_message>
72. Why a Learning Rate?
</commit_message>
<xml_diff>
--- a/resources/mse_graph.xlsx
+++ b/resources/mse_graph.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noah/Documents/study/study_codes/udemy/machine-learning-js-stephen/machine-learning-js-stephen-git/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC328862-739A-D04C-B78A-4A66A961013D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB53765A-0CBE-FA47-ACCD-286ED7B01F01}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1680" yWindow="-20940" windowWidth="29980" windowHeight="18940" xr2:uid="{4090F69A-B87C-A848-B205-CF8351D4CAAD}"/>
+    <workbookView xWindow="-1680" yWindow="-20940" windowWidth="29980" windowHeight="18940" activeTab="1" xr2:uid="{4090F69A-B87C-A848-B205-CF8351D4CAAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Gradient Descent" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Guess for B</t>
   </si>
@@ -52,6 +53,15 @@
   </si>
   <si>
     <t>How Much To Adjust B</t>
+  </si>
+  <si>
+    <t>to see the chart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try other </t>
+  </si>
+  <si>
+    <t>learning rate</t>
   </si>
 </sst>
 </file>
@@ -87,7 +97,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -104,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -115,10 +125,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,7 +732,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>60132</c:v>
+                  <c:v>60621</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>55352</c:v>
@@ -1037,6 +1048,533 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Gradient Descent'!$E$2:$E$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>205.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>229.32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>238.72800000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>242.49119999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>243.99647999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>244.598592</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>244.83943679999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>244.93577471999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>244.97430988799999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>244.98972395519999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>244.99588958208</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>244.998355832832</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>244.9993423331328</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>244.99973693325313</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>244.99989477330126</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>244.9999579093205</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>244.99998316372819</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>244.99999326549127</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>244.99999730619652</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>244.9999989224786</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>244.99999956899143</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>244.99999982759658</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>244.99999993103864</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>244.99999997241545</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>244.99999998896618</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>244.99999999558648</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>244.99999999823459</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>244.99999999929383</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>244.99999999971755</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>244.99999999988702</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>244.99999999995481</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>244.99999999998192</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>244.99999999999278</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>244.9999999999971</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>244.99999999999883</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>244.99999999999955</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>244.99999999999983</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>244.99999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Gradient Descent'!$F$2:$F$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>60621</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2132.6399999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>841.86240000000032</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>635.33798399999989</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>602.29407744000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>597.00705239039996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>596.16112838246397</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>596.02578054119431</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>596.00412488659106</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>596.00065998185448</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>596.00010559709665</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>596.00001689553551</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>596.00000270328553</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>596.00000043252578</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>596.00000006920413</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>596.00000001107264</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>596.0000000017717</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>596.00000000028342</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>596.00000000004536</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>596.00000000000728</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>596.00000000000125</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>596.00000000000011</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>596</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>595.99999999999989</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>596.00000000000011</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>595.99999999999989</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>595.99999999999989</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>595.99999999999989</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>596</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>596</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>595.99999999999989</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>596.00000000000011</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>596</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>596</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>596.00000000000011</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>596.00000000000011</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>596</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>596.00000000000011</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>596</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-982E-EE40-BD0F-3876FF9D3CD9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1837505072"/>
+        <c:axId val="147014415"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1837505072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="147014415"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="147014415"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1837505072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1117,6 +1655,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2149,20 +2727,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2190,15 +3284,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>615950</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2218,6 +3312,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04ACE903-5BC0-D849-8F8D-2EC0B71C38D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2523,979 +3658,1396 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD848182-8EBD-094B-9D79-4F6A3B7DE717}">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>800</v>
       </c>
       <c r="B2" s="1">
         <v>200</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="5">
-        <f>2 * ((J2-$B$2) + (J2-$B$3) + (J2-$B$4) + (J2-$B$5) + (J2-$B$6) + (J2-$B$7)) / 6</f>
-        <v>-490</v>
-      </c>
-      <c r="L2">
-        <f>K2*$G$3</f>
-        <v>-147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>950</v>
       </c>
       <c r="B3" s="1">
         <v>230</v>
       </c>
-      <c r="G3">
-        <v>0.3</v>
-      </c>
-      <c r="J3">
-        <f>J2-L2</f>
-        <v>147</v>
-      </c>
-      <c r="K3" s="5">
-        <f>2 * ((J3-$B$2) + (J3-$B$3) + (J3-$B$4) + (J3-$B$5) + (J3-$B$6) + (J3-$B$7)) / 6</f>
-        <v>-196</v>
-      </c>
-      <c r="L3">
-        <f>K3*$G$3</f>
-        <v>-58.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1040</v>
       </c>
       <c r="B4" s="1">
         <v>245</v>
       </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J27" si="0">J3-L3</f>
-        <v>205.8</v>
-      </c>
-      <c r="K4" s="5">
-        <f t="shared" ref="K4:K41" si="1">2 * ((J4-$B$2) + (J4-$B$3) + (J4-$B$4) + (J4-$B$5) + (J4-$B$6) + (J4-$B$7)) / 6</f>
-        <v>-78.399999999999977</v>
-      </c>
-      <c r="L4">
-        <f t="shared" ref="L4:L41" si="2">K4*$G$3</f>
-        <v>-23.519999999999992</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1120</v>
       </c>
       <c r="B5" s="1">
         <v>274</v>
       </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>229.32</v>
-      </c>
-      <c r="K5" s="5">
-        <f t="shared" si="1"/>
-        <v>-31.360000000000014</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="2"/>
-        <v>-9.408000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1250</v>
       </c>
       <c r="B6" s="1">
         <v>259</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>238.72800000000001</v>
-      </c>
-      <c r="K6" s="5">
-        <f t="shared" si="1"/>
-        <v>-12.543999999999983</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="2"/>
-        <v>-3.7631999999999945</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>1350</v>
       </c>
       <c r="B7" s="1">
         <v>262</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>242.49119999999999</v>
-      </c>
-      <c r="K7" s="5">
-        <f t="shared" si="1"/>
-        <v>-5.0176000000000158</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="2"/>
-        <v>-1.5052800000000046</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>243.99647999999999</v>
-      </c>
-      <c r="K8" s="5">
-        <f t="shared" si="1"/>
-        <v>-2.0070400000000177</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="2"/>
-        <v>-0.60211200000000531</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>244.598592</v>
-      </c>
-      <c r="K9" s="5">
-        <f t="shared" si="1"/>
-        <v>-0.80281600000000708</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="2"/>
-        <v>-0.24084480000000211</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>1</v>
       </c>
       <c r="B10" s="3">
-        <f t="shared" ref="B10:B49" si="3">(($A10-$B$2)^2+($A10-$B$3)^2+($A10-$B$4)^2+($A10-$B$5)^2+($A10-$B$6)^2+($A10-$B$7)^2) / 6</f>
-        <v>60132</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>244.83943679999999</v>
-      </c>
-      <c r="K10" s="5">
-        <f t="shared" si="1"/>
-        <v>-0.32112640000002557</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="2"/>
-        <v>-9.6337920000007668E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <f>'Gradient Descent'!F2</f>
+        <v>60621</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <f>A10+10</f>
         <v>11</v>
       </c>
       <c r="B11" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="B10:B49" si="0">(($A11-$B$2)^2+($A11-$B$3)^2+($A11-$B$4)^2+($A11-$B$5)^2+($A11-$B$6)^2+($A11-$B$7)^2) / 6</f>
         <v>55352</v>
       </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>244.93577471999998</v>
-      </c>
-      <c r="K11" s="5">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <f t="shared" ref="A12:A40" si="1">A11+10</f>
+        <v>21</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
+        <v>50772</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
         <f t="shared" si="1"/>
-        <v>-0.12845056000003297</v>
-      </c>
-      <c r="L11">
+        <v>31</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>46392</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>42212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>38232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="0"/>
+        <v>34452</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" si="0"/>
+        <v>30872</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" si="0"/>
+        <v>27492</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" si="0"/>
+        <v>24312</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="0"/>
+        <v>21332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" si="0"/>
+        <v>18552</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="0"/>
+        <v>15972</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" si="0"/>
+        <v>13592</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <f t="shared" si="1"/>
+        <v>141</v>
+      </c>
+      <c r="B24" s="3">
+        <f t="shared" si="0"/>
+        <v>11412</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <f t="shared" si="1"/>
+        <v>151</v>
+      </c>
+      <c r="B25" s="3">
+        <f t="shared" si="0"/>
+        <v>9432</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <f t="shared" si="1"/>
+        <v>161</v>
+      </c>
+      <c r="B26" s="3">
+        <f t="shared" si="0"/>
+        <v>7652</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <f t="shared" si="1"/>
+        <v>171</v>
+      </c>
+      <c r="B27" s="3">
+        <f t="shared" si="0"/>
+        <v>6072</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <f t="shared" si="1"/>
+        <v>181</v>
+      </c>
+      <c r="B28" s="3">
+        <f t="shared" si="0"/>
+        <v>4692</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <f t="shared" si="1"/>
+        <v>191</v>
+      </c>
+      <c r="B29" s="3">
+        <f t="shared" si="0"/>
+        <v>3512</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <f t="shared" si="1"/>
+        <v>201</v>
+      </c>
+      <c r="B30" s="3">
+        <f t="shared" si="0"/>
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <f t="shared" si="1"/>
+        <v>211</v>
+      </c>
+      <c r="B31" s="3">
+        <f t="shared" si="0"/>
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <f t="shared" si="1"/>
+        <v>221</v>
+      </c>
+      <c r="B32" s="3">
+        <f t="shared" si="0"/>
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <f t="shared" si="1"/>
+        <v>231</v>
+      </c>
+      <c r="B33" s="3">
+        <f t="shared" si="0"/>
+        <v>792</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <f t="shared" si="1"/>
+        <v>241</v>
+      </c>
+      <c r="B34" s="3">
+        <f t="shared" si="0"/>
+        <v>612</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="B35" s="3">
+        <f t="shared" si="0"/>
+        <v>632</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <f t="shared" si="1"/>
+        <v>261</v>
+      </c>
+      <c r="B36" s="3">
+        <f t="shared" si="0"/>
+        <v>852</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <f t="shared" si="1"/>
+        <v>271</v>
+      </c>
+      <c r="B37" s="3">
+        <f t="shared" si="0"/>
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <f t="shared" si="1"/>
+        <v>281</v>
+      </c>
+      <c r="B38" s="3">
+        <f t="shared" si="0"/>
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <f t="shared" si="1"/>
+        <v>291</v>
+      </c>
+      <c r="B39" s="3">
+        <f t="shared" si="0"/>
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <f t="shared" si="1"/>
+        <v>301</v>
+      </c>
+      <c r="B40" s="3">
+        <f t="shared" si="0"/>
+        <v>3732</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <f t="shared" ref="A41:A49" si="2">A40+10</f>
+        <v>311</v>
+      </c>
+      <c r="B41" s="3">
+        <f t="shared" si="0"/>
+        <v>4952</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
         <f t="shared" si="2"/>
-        <v>-3.853516800000989E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <f t="shared" ref="A12:A40" si="4">A11+10</f>
-        <v>21</v>
-      </c>
-      <c r="B12" s="3">
-        <f t="shared" si="3"/>
-        <v>50772</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>244.97430988799999</v>
-      </c>
-      <c r="K12" s="5">
-        <f t="shared" si="1"/>
-        <v>-5.1380224000013186E-2</v>
-      </c>
-      <c r="L12">
+        <v>321</v>
+      </c>
+      <c r="B42" s="3">
+        <f t="shared" si="0"/>
+        <v>6372</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
         <f t="shared" si="2"/>
-        <v>-1.5414067200003954E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <f t="shared" si="4"/>
-        <v>31</v>
-      </c>
-      <c r="B13" s="3">
-        <f t="shared" si="3"/>
-        <v>46392</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>244.98972395519999</v>
-      </c>
-      <c r="K13" s="5">
-        <f t="shared" si="1"/>
-        <v>-2.0552089600016643E-2</v>
-      </c>
-      <c r="L13">
+        <v>331</v>
+      </c>
+      <c r="B43" s="3">
+        <f t="shared" si="0"/>
+        <v>7992</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
         <f t="shared" si="2"/>
-        <v>-6.1656268800049929E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <f t="shared" si="4"/>
-        <v>41</v>
-      </c>
-      <c r="B14" s="3">
-        <f t="shared" si="3"/>
-        <v>42212</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>244.99588958208</v>
-      </c>
-      <c r="K14" s="5">
-        <f t="shared" si="1"/>
-        <v>-8.2208358400066572E-3</v>
-      </c>
-      <c r="L14">
+        <v>341</v>
+      </c>
+      <c r="B44" s="3">
+        <f t="shared" si="0"/>
+        <v>9812</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
         <f t="shared" si="2"/>
-        <v>-2.4662507520019973E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <f t="shared" si="4"/>
-        <v>51</v>
-      </c>
-      <c r="B15" s="3">
-        <f t="shared" si="3"/>
-        <v>38232</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
-        <v>244.998355832832</v>
-      </c>
-      <c r="K15" s="5">
-        <f t="shared" si="1"/>
-        <v>-3.2883343359912942E-3</v>
-      </c>
-      <c r="L15">
+        <v>351</v>
+      </c>
+      <c r="B45" s="3">
+        <f t="shared" si="0"/>
+        <v>11832</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
         <f t="shared" si="2"/>
-        <v>-9.8650030079738826E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <f t="shared" si="4"/>
-        <v>61</v>
-      </c>
-      <c r="B16" s="3">
-        <f t="shared" si="3"/>
-        <v>34452</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="0"/>
-        <v>244.9993423331328</v>
-      </c>
-      <c r="K16" s="5">
-        <f t="shared" si="1"/>
-        <v>-1.3153337343965177E-3</v>
-      </c>
-      <c r="L16">
+        <v>361</v>
+      </c>
+      <c r="B46" s="3">
+        <f t="shared" si="0"/>
+        <v>14052</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
         <f t="shared" si="2"/>
-        <v>-3.9460012031895532E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <f t="shared" si="4"/>
-        <v>71</v>
-      </c>
-      <c r="B17" s="3">
-        <f t="shared" si="3"/>
-        <v>30872</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="0"/>
-        <v>244.99973693325313</v>
-      </c>
-      <c r="K17" s="5">
-        <f t="shared" si="1"/>
-        <v>-5.2613349373586971E-4</v>
-      </c>
-      <c r="L17">
+        <v>371</v>
+      </c>
+      <c r="B47" s="3">
+        <f t="shared" si="0"/>
+        <v>16472</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
         <f t="shared" si="2"/>
-        <v>-1.578400481207609E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <f t="shared" si="4"/>
-        <v>81</v>
-      </c>
-      <c r="B18" s="3">
-        <f t="shared" si="3"/>
-        <v>27492</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="0"/>
-        <v>244.99989477330126</v>
-      </c>
-      <c r="K18" s="5">
-        <f t="shared" si="1"/>
-        <v>-2.1045339747161051E-4</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="2"/>
-        <v>-6.3136019241483149E-5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <f t="shared" si="4"/>
-        <v>91</v>
-      </c>
-      <c r="B19" s="3">
-        <f t="shared" si="3"/>
-        <v>24312</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="0"/>
-        <v>244.9999579093205</v>
-      </c>
-      <c r="K19" s="5">
-        <f t="shared" si="1"/>
-        <v>-8.418135900001289E-5</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="2"/>
-        <v>-2.5254407700003866E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <f t="shared" si="4"/>
-        <v>101</v>
-      </c>
-      <c r="B20" s="3">
-        <f t="shared" si="3"/>
-        <v>21332</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="0"/>
-        <v>244.99998316372819</v>
-      </c>
-      <c r="K20" s="5">
-        <f t="shared" si="1"/>
-        <v>-3.3672543622742523E-5</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="2"/>
-        <v>-1.0101763086822757E-5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <f t="shared" si="4"/>
-        <v>111</v>
-      </c>
-      <c r="B21" s="3">
-        <f t="shared" si="3"/>
-        <v>18552</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="0"/>
-        <v>244.99999326549127</v>
-      </c>
-      <c r="K21" s="5">
-        <f t="shared" si="1"/>
-        <v>-1.3469017460465693E-5</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="2"/>
-        <v>-4.0407052381397078E-6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <f t="shared" si="4"/>
-        <v>121</v>
-      </c>
-      <c r="B22" s="3">
-        <f t="shared" si="3"/>
-        <v>15972</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="0"/>
-        <v>244.99999730619652</v>
-      </c>
-      <c r="K22" s="5">
-        <f t="shared" si="1"/>
-        <v>-5.3876069614489097E-6</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="2"/>
-        <v>-1.6162820884346729E-6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <f t="shared" si="4"/>
-        <v>131</v>
-      </c>
-      <c r="B23" s="3">
-        <f t="shared" si="3"/>
-        <v>13592</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="0"/>
-        <v>244.9999989224786</v>
-      </c>
-      <c r="K23" s="5">
-        <f t="shared" si="1"/>
-        <v>-2.1550428073169314E-6</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="2"/>
-        <v>-6.4651284219507939E-7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
-        <f t="shared" si="4"/>
-        <v>141</v>
-      </c>
-      <c r="B24" s="3">
-        <f t="shared" si="3"/>
-        <v>11412</v>
-      </c>
-      <c r="J24" s="8">
-        <f t="shared" si="0"/>
-        <v>244.99999956899143</v>
-      </c>
-      <c r="K24" s="9">
-        <f t="shared" si="1"/>
-        <v>-8.6201714566414012E-7</v>
-      </c>
-      <c r="L24" s="8">
-        <f t="shared" si="2"/>
-        <v>-2.5860514369924202E-7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <f t="shared" si="4"/>
-        <v>151</v>
-      </c>
-      <c r="B25" s="3">
-        <f t="shared" si="3"/>
-        <v>9432</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="0"/>
-        <v>244.99999982759658</v>
-      </c>
-      <c r="K25" s="5">
-        <f t="shared" si="1"/>
-        <v>-3.448068355282885E-7</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="2"/>
-        <v>-1.0344205065848655E-7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
-        <f t="shared" si="4"/>
-        <v>161</v>
-      </c>
-      <c r="B26" s="3">
-        <f t="shared" si="3"/>
-        <v>7652</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="0"/>
-        <v>244.99999993103864</v>
-      </c>
-      <c r="K26" s="5">
-        <f t="shared" si="1"/>
-        <v>-1.3792271147394786E-7</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="2"/>
-        <v>-4.1376813442184356E-8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
-        <f t="shared" si="4"/>
-        <v>171</v>
-      </c>
-      <c r="B27" s="3">
-        <f t="shared" si="3"/>
-        <v>6072</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="0"/>
-        <v>244.99999997241545</v>
-      </c>
-      <c r="K27" s="5">
-        <f t="shared" si="1"/>
-        <v>-5.5169095958262915E-8</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="2"/>
-        <v>-1.6550728787478874E-8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
-        <f t="shared" si="4"/>
-        <v>181</v>
-      </c>
-      <c r="B28" s="3">
-        <f t="shared" si="3"/>
-        <v>4692</v>
-      </c>
-      <c r="J28">
-        <f>J27-L27</f>
-        <v>244.99999998896618</v>
-      </c>
-      <c r="K28" s="5">
-        <f>2 * ((J28-$B$2) + (J28-$B$3) + (J28-$B$4) + (J28-$B$5) + (J28-$B$6) + (J28-$B$7)) / 6</f>
-        <v>-2.2067638383305166E-8</v>
-      </c>
-      <c r="L28">
-        <f>K28*$G$3</f>
-        <v>-6.6202915149915494E-9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <f t="shared" si="4"/>
-        <v>191</v>
-      </c>
-      <c r="B29" s="3">
-        <f t="shared" si="3"/>
-        <v>3512</v>
-      </c>
-      <c r="J29">
-        <f t="shared" ref="J29:J33" si="5">J28-L28</f>
-        <v>244.99999999558648</v>
-      </c>
-      <c r="K29" s="5">
-        <f t="shared" si="1"/>
-        <v>-8.8270439846382942E-9</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="2"/>
-        <v>-2.6481131953914882E-9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <f t="shared" si="4"/>
-        <v>201</v>
-      </c>
-      <c r="B30" s="3">
-        <f t="shared" si="3"/>
-        <v>2532</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="5"/>
-        <v>244.99999999823459</v>
-      </c>
-      <c r="K30" s="5">
-        <f t="shared" si="1"/>
-        <v>-3.5308289625390898E-9</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="2"/>
-        <v>-1.059248688761727E-9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
-        <f t="shared" si="4"/>
-        <v>211</v>
-      </c>
-      <c r="B31" s="3">
-        <f t="shared" si="3"/>
-        <v>1752</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="5"/>
-        <v>244.99999999929383</v>
-      </c>
-      <c r="K31" s="5">
-        <f t="shared" si="1"/>
-        <v>-1.4123315850156359E-9</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="2"/>
-        <v>-4.2369947550469074E-10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
-        <f t="shared" si="4"/>
-        <v>221</v>
-      </c>
-      <c r="B32" s="3">
-        <f t="shared" si="3"/>
-        <v>1172</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="5"/>
-        <v>244.99999999971755</v>
-      </c>
-      <c r="K32" s="5">
-        <f t="shared" si="1"/>
-        <v>-5.6490989663871005E-10</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="2"/>
-        <v>-1.6947296899161302E-10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
-        <f t="shared" si="4"/>
-        <v>231</v>
-      </c>
-      <c r="B33" s="3">
-        <f t="shared" si="3"/>
-        <v>792</v>
-      </c>
-      <c r="J33">
-        <f t="shared" si="5"/>
-        <v>244.99999999988702</v>
-      </c>
-      <c r="K33" s="5">
-        <f t="shared" si="1"/>
-        <v>-2.2595258997171186E-10</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="2"/>
-        <v>-6.7785776991513558E-11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
-        <f t="shared" si="4"/>
-        <v>241</v>
-      </c>
-      <c r="B34" s="3">
-        <f t="shared" si="3"/>
-        <v>612</v>
-      </c>
-      <c r="J34">
-        <f>J33-L33</f>
-        <v>244.99999999995481</v>
-      </c>
-      <c r="K34" s="5">
-        <f>2 * ((J34-$B$2) + (J34-$B$3) + (J34-$B$4) + (J34-$B$5) + (J34-$B$6) + (J34-$B$7)) / 6</f>
-        <v>-9.0381035988684744E-11</v>
-      </c>
-      <c r="L34">
-        <f>K34*$G$3</f>
-        <v>-2.7114310796605423E-11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
-        <f t="shared" si="4"/>
-        <v>251</v>
-      </c>
-      <c r="B35" s="3">
-        <f t="shared" si="3"/>
-        <v>632</v>
-      </c>
-      <c r="J35">
-        <f t="shared" ref="J35" si="6">J34-L34</f>
-        <v>244.99999999998192</v>
-      </c>
-      <c r="K35" s="5">
-        <f t="shared" si="1"/>
-        <v>-3.6152414395473897E-11</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="2"/>
-        <v>-1.0845724318642168E-11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
-        <f t="shared" si="4"/>
-        <v>261</v>
-      </c>
-      <c r="B36" s="3">
-        <f t="shared" si="3"/>
-        <v>852</v>
-      </c>
-      <c r="J36">
-        <f t="shared" ref="J36:J41" si="7">J35-L35</f>
-        <v>244.99999999999278</v>
-      </c>
-      <c r="K36" s="5">
-        <f t="shared" si="1"/>
-        <v>-1.4438228390645236E-11</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="2"/>
-        <v>-4.3314685171935709E-12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
-        <f t="shared" si="4"/>
-        <v>271</v>
-      </c>
-      <c r="B37" s="3">
-        <f t="shared" si="3"/>
-        <v>1272</v>
-      </c>
-      <c r="J37">
-        <f t="shared" si="7"/>
-        <v>244.9999999999971</v>
-      </c>
-      <c r="K37" s="5">
-        <f t="shared" si="1"/>
-        <v>-5.7980287238024175E-12</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="2"/>
-        <v>-1.7394086171407251E-12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
-        <f t="shared" si="4"/>
-        <v>281</v>
-      </c>
-      <c r="B38" s="3">
-        <f t="shared" si="3"/>
-        <v>1892</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="7"/>
-        <v>244.99999999999883</v>
-      </c>
-      <c r="K38" s="5">
-        <f t="shared" si="1"/>
-        <v>-2.3305801732931286E-12</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="2"/>
-        <v>-6.9917405198793852E-13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
-        <f t="shared" si="4"/>
-        <v>291</v>
-      </c>
-      <c r="B39" s="3">
-        <f t="shared" si="3"/>
-        <v>2712</v>
-      </c>
-      <c r="J39">
-        <f t="shared" si="7"/>
-        <v>244.99999999999955</v>
-      </c>
-      <c r="K39" s="5">
-        <f t="shared" si="1"/>
-        <v>-9.0949470177292824E-13</v>
-      </c>
-      <c r="L39">
-        <f t="shared" si="2"/>
-        <v>-2.7284841053187846E-13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
-        <f t="shared" si="4"/>
-        <v>301</v>
-      </c>
-      <c r="B40" s="3">
-        <f t="shared" si="3"/>
-        <v>3732</v>
-      </c>
-      <c r="J40">
-        <f t="shared" si="7"/>
-        <v>244.99999999999983</v>
-      </c>
-      <c r="K40" s="5">
-        <f t="shared" si="1"/>
-        <v>-3.4106051316484809E-13</v>
-      </c>
-      <c r="L40">
-        <f t="shared" si="2"/>
-        <v>-1.0231815394945442E-13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
-        <f t="shared" ref="A41:A49" si="8">A40+10</f>
-        <v>311</v>
-      </c>
-      <c r="B41" s="3">
-        <f t="shared" si="3"/>
-        <v>4952</v>
-      </c>
-      <c r="J41">
-        <f t="shared" si="7"/>
-        <v>244.99999999999994</v>
-      </c>
-      <c r="K41" s="5">
-        <f t="shared" si="1"/>
-        <v>-1.1368683772161603E-13</v>
-      </c>
-      <c r="L41">
-        <f t="shared" si="2"/>
-        <v>-3.4106051316484808E-14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
-        <f t="shared" si="8"/>
-        <v>321</v>
-      </c>
-      <c r="B42" s="3">
-        <f t="shared" si="3"/>
-        <v>6372</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="2">
-        <f t="shared" si="8"/>
-        <v>331</v>
-      </c>
-      <c r="B43" s="3">
-        <f t="shared" si="3"/>
-        <v>7992</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
-        <f t="shared" si="8"/>
-        <v>341</v>
-      </c>
-      <c r="B44" s="3">
-        <f t="shared" si="3"/>
-        <v>9812</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="2">
-        <f t="shared" si="8"/>
-        <v>351</v>
-      </c>
-      <c r="B45" s="3">
-        <f t="shared" si="3"/>
-        <v>11832</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
-        <f t="shared" si="8"/>
-        <v>361</v>
-      </c>
-      <c r="B46" s="3">
-        <f t="shared" si="3"/>
-        <v>14052</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" s="2">
-        <f t="shared" si="8"/>
-        <v>371</v>
-      </c>
-      <c r="B47" s="3">
-        <f t="shared" si="3"/>
-        <v>16472</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
-        <f t="shared" si="8"/>
         <v>381</v>
       </c>
       <c r="B48" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>19092</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>391</v>
       </c>
       <c r="B49" s="3">
+        <f t="shared" si="0"/>
+        <v>21912</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1F2E40-F65D-B748-9EBC-90B3D8E3A982}">
+  <dimension ref="A1:H49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>800</v>
+      </c>
+      <c r="B2" s="1">
+        <v>200</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>((E2-$B$2)^2+(E2-$B$3)^2+(E2-$B$4)^2+(E2-$B$5)^2+(E2-$B$6)^2+(E2-$B$7)^2) / 6</f>
+        <v>60621</v>
+      </c>
+      <c r="G2" s="5">
+        <f>2 * ((E2-$B$2) + (E2-$B$3) + (E2-$B$4) + (E2-$B$5) + (E2-$B$6) + (E2-$B$7)) / 6</f>
+        <v>-490</v>
+      </c>
+      <c r="H2">
+        <f>G2*$B$10</f>
+        <v>-147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>950</v>
+      </c>
+      <c r="B3" s="1">
+        <v>230</v>
+      </c>
+      <c r="E3">
+        <f>E2-H2</f>
+        <v>147</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F41" si="0">((E3-$B$2)^2+(E3-$B$3)^2+(E3-$B$4)^2+(E3-$B$5)^2+(E3-$B$6)^2+(E3-$B$7)^2) / 6</f>
+        <v>10200</v>
+      </c>
+      <c r="G3" s="5">
+        <f>2 * ((E3-$B$2) + (E3-$B$3) + (E3-$B$4) + (E3-$B$5) + (E3-$B$6) + (E3-$B$7)) / 6</f>
+        <v>-196</v>
+      </c>
+      <c r="H3">
+        <f>G3*$B$10</f>
+        <v>-58.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1040</v>
+      </c>
+      <c r="B4" s="1">
+        <v>245</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E27" si="1">E3-H3</f>
+        <v>205.8</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>2132.6399999999994</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" ref="G4:G41" si="2">2 * ((E4-$B$2) + (E4-$B$3) + (E4-$B$4) + (E4-$B$5) + (E4-$B$6) + (E4-$B$7)) / 6</f>
+        <v>-78.399999999999977</v>
+      </c>
+      <c r="H4">
+        <f>G4*$B$10</f>
+        <v>-23.519999999999992</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>1120</v>
+      </c>
+      <c r="B5" s="1">
+        <v>274</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>229.32</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>841.86240000000032</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" si="2"/>
+        <v>-31.360000000000014</v>
+      </c>
+      <c r="H5">
+        <f>G5*$B$10</f>
+        <v>-9.408000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>1250</v>
+      </c>
+      <c r="B6" s="1">
+        <v>259</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>238.72800000000001</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>635.33798399999989</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="2"/>
+        <v>-12.543999999999983</v>
+      </c>
+      <c r="H6">
+        <f>G6*$B$10</f>
+        <v>-3.7631999999999945</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>1350</v>
+      </c>
+      <c r="B7" s="1">
+        <v>262</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>242.49119999999999</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>602.29407744000002</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="2"/>
+        <v>-5.0176000000000158</v>
+      </c>
+      <c r="H7">
+        <f>G7*$B$10</f>
+        <v>-1.5052800000000046</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>243.99647999999999</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>597.00705239039996</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.0070400000000177</v>
+      </c>
+      <c r="H8">
+        <f>G8*$B$10</f>
+        <v>-0.60211200000000531</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>244.598592</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>596.16112838246397</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="2"/>
+        <v>-0.80281600000000708</v>
+      </c>
+      <c r="H9">
+        <f>G9*$B$10</f>
+        <v>-0.24084480000000211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>244.83943679999999</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>596.02578054119431</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="2"/>
+        <v>-0.32112640000002557</v>
+      </c>
+      <c r="H10">
+        <f>G10*$B$10</f>
+        <v>-9.6337920000007668E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>0.1</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>244.93577471999998</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>596.00412488659106</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" si="2"/>
+        <v>-0.12845056000003297</v>
+      </c>
+      <c r="H11">
+        <f>G11*$B$10</f>
+        <v>-3.853516800000989E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>0.3</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>244.97430988799999</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>596.00065998185448</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="2"/>
+        <v>-5.1380224000013186E-2</v>
+      </c>
+      <c r="H12">
+        <f>G12*$B$10</f>
+        <v>-1.5414067200003954E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>0.9</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>244.98972395519999</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>596.00010559709665</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.0552089600016643E-2</v>
+      </c>
+      <c r="H13">
+        <f>G13*$B$10</f>
+        <v>-6.1656268800049929E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>0.98</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>244.99588958208</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>596.00001689553551</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" si="2"/>
+        <v>-8.2208358400066572E-3</v>
+      </c>
+      <c r="H14">
+        <f>G14*$B$10</f>
+        <v>-2.4662507520019973E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>244.998355832832</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>596.00000270328553</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" si="2"/>
+        <v>-3.2883343359912942E-3</v>
+      </c>
+      <c r="H15">
+        <f>G15*$B$10</f>
+        <v>-9.8650030079738826E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="3"/>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>244.9993423331328</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>596.00000043252578</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.3153337343965177E-3</v>
+      </c>
+      <c r="H16">
+        <f>G16*$B$10</f>
+        <v>-3.9460012031895532E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>244.99973693325313</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>596.00000006920413</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="2"/>
+        <v>-5.2613349373586971E-4</v>
+      </c>
+      <c r="H17">
+        <f>G17*$B$10</f>
+        <v>-1.578400481207609E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>244.99989477330126</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>596.00000001107264</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.1045339747161051E-4</v>
+      </c>
+      <c r="H18">
+        <f>G18*$B$10</f>
+        <v>-6.3136019241483149E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>244.9999579093205</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>596.0000000017717</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="2"/>
+        <v>-8.418135900001289E-5</v>
+      </c>
+      <c r="H19">
+        <f>G19*$B$10</f>
+        <v>-2.5254407700003866E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>244.99998316372819</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>596.00000000028342</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" si="2"/>
+        <v>-3.3672543622742523E-5</v>
+      </c>
+      <c r="H20">
+        <f>G20*$B$10</f>
+        <v>-1.0101763086822757E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>244.99999326549127</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>596.00000000004536</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.3469017460465693E-5</v>
+      </c>
+      <c r="H21">
+        <f>G21*$B$10</f>
+        <v>-4.0407052381397078E-6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>244.99999730619652</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>596.00000000000728</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" si="2"/>
+        <v>-5.3876069614489097E-6</v>
+      </c>
+      <c r="H22">
+        <f>G22*$B$10</f>
+        <v>-1.6162820884346729E-6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>244.9999989224786</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>596.00000000000125</v>
+      </c>
+      <c r="G23" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.1550428073169314E-6</v>
+      </c>
+      <c r="H23">
+        <f>G23*$B$10</f>
+        <v>-6.4651284219507939E-7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="E24" s="8">
+        <f t="shared" si="1"/>
+        <v>244.99999956899143</v>
+      </c>
+      <c r="F24" s="8">
+        <f t="shared" si="0"/>
+        <v>596.00000000000011</v>
+      </c>
+      <c r="G24" s="9">
+        <f t="shared" si="2"/>
+        <v>-8.6201714566414012E-7</v>
+      </c>
+      <c r="H24" s="8">
+        <f>G24*$B$10</f>
+        <v>-2.5860514369924202E-7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>244.99999982759658</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>596</v>
+      </c>
+      <c r="G25" s="5">
+        <f t="shared" si="2"/>
+        <v>-3.448068355282885E-7</v>
+      </c>
+      <c r="H25">
+        <f>G25*$B$10</f>
+        <v>-1.0344205065848655E-7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>244.99999993103864</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>595.99999999999989</v>
+      </c>
+      <c r="G26" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.3792271147394786E-7</v>
+      </c>
+      <c r="H26">
+        <f>G26*$B$10</f>
+        <v>-4.1376813442184356E-8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>244.99999997241545</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>596.00000000000011</v>
+      </c>
+      <c r="G27" s="5">
+        <f t="shared" si="2"/>
+        <v>-5.5169095958262915E-8</v>
+      </c>
+      <c r="H27">
+        <f>G27*$B$10</f>
+        <v>-1.6550728787478874E-8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="E28">
+        <f>E27-H27</f>
+        <v>244.99999998896618</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>595.99999999999989</v>
+      </c>
+      <c r="G28" s="5">
+        <f>2 * ((E28-$B$2) + (E28-$B$3) + (E28-$B$4) + (E28-$B$5) + (E28-$B$6) + (E28-$B$7)) / 6</f>
+        <v>-2.2067638383305166E-8</v>
+      </c>
+      <c r="H28">
+        <f>G28*$B$10</f>
+        <v>-6.6202915149915494E-9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="E29">
+        <f t="shared" ref="E29:E33" si="3">E28-H28</f>
+        <v>244.99999999558648</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>595.99999999999989</v>
+      </c>
+      <c r="G29" s="5">
+        <f t="shared" si="2"/>
+        <v>-8.8270439846382942E-9</v>
+      </c>
+      <c r="H29">
+        <f>G29*$B$10</f>
+        <v>-2.6481131953914882E-9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="E30">
         <f t="shared" si="3"/>
-        <v>21912</v>
-      </c>
+        <v>244.99999999823459</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>595.99999999999989</v>
+      </c>
+      <c r="G30" s="5">
+        <f t="shared" si="2"/>
+        <v>-3.5308289625390898E-9</v>
+      </c>
+      <c r="H30">
+        <f>G30*$B$10</f>
+        <v>-1.059248688761727E-9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="E31">
+        <f t="shared" si="3"/>
+        <v>244.99999999929383</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>596</v>
+      </c>
+      <c r="G31" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.4123315850156359E-9</v>
+      </c>
+      <c r="H31">
+        <f>G31*$B$10</f>
+        <v>-4.2369947550469074E-10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="E32">
+        <f t="shared" si="3"/>
+        <v>244.99999999971755</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>596</v>
+      </c>
+      <c r="G32" s="5">
+        <f t="shared" si="2"/>
+        <v>-5.6490989663871005E-10</v>
+      </c>
+      <c r="H32">
+        <f>G32*$B$10</f>
+        <v>-1.6947296899161302E-10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="E33">
+        <f t="shared" si="3"/>
+        <v>244.99999999988702</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>595.99999999999989</v>
+      </c>
+      <c r="G33" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.2595258997171186E-10</v>
+      </c>
+      <c r="H33">
+        <f>G33*$B$10</f>
+        <v>-6.7785776991513558E-11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="E34">
+        <f>E33-H33</f>
+        <v>244.99999999995481</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>596.00000000000011</v>
+      </c>
+      <c r="G34" s="5">
+        <f>2 * ((E34-$B$2) + (E34-$B$3) + (E34-$B$4) + (E34-$B$5) + (E34-$B$6) + (E34-$B$7)) / 6</f>
+        <v>-9.0381035988684744E-11</v>
+      </c>
+      <c r="H34">
+        <f>G34*$B$10</f>
+        <v>-2.7114310796605423E-11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="E35">
+        <f t="shared" ref="E35:E41" si="4">E34-H34</f>
+        <v>244.99999999998192</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>596</v>
+      </c>
+      <c r="G35" s="5">
+        <f t="shared" si="2"/>
+        <v>-3.6152414395473897E-11</v>
+      </c>
+      <c r="H35">
+        <f>G35*$B$10</f>
+        <v>-1.0845724318642168E-11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="E36">
+        <f t="shared" si="4"/>
+        <v>244.99999999999278</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>596</v>
+      </c>
+      <c r="G36" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.4438228390645236E-11</v>
+      </c>
+      <c r="H36">
+        <f>G36*$B$10</f>
+        <v>-4.3314685171935709E-12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="3"/>
+      <c r="E37">
+        <f t="shared" si="4"/>
+        <v>244.9999999999971</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>596.00000000000011</v>
+      </c>
+      <c r="G37" s="5">
+        <f t="shared" si="2"/>
+        <v>-5.7980287238024175E-12</v>
+      </c>
+      <c r="H37">
+        <f>G37*$B$10</f>
+        <v>-1.7394086171407251E-12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="3"/>
+      <c r="E38">
+        <f t="shared" si="4"/>
+        <v>244.99999999999883</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>596.00000000000011</v>
+      </c>
+      <c r="G38" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.3305801732931286E-12</v>
+      </c>
+      <c r="H38">
+        <f>G38*$B$10</f>
+        <v>-6.9917405198793852E-13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="E39">
+        <f t="shared" si="4"/>
+        <v>244.99999999999955</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>596</v>
+      </c>
+      <c r="G39" s="5">
+        <f t="shared" si="2"/>
+        <v>-9.0949470177292824E-13</v>
+      </c>
+      <c r="H39">
+        <f>G39*$B$10</f>
+        <v>-2.7284841053187846E-13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="3"/>
+      <c r="E40">
+        <f t="shared" si="4"/>
+        <v>244.99999999999983</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>596.00000000000011</v>
+      </c>
+      <c r="G40" s="5">
+        <f t="shared" si="2"/>
+        <v>-3.4106051316484809E-13</v>
+      </c>
+      <c r="H40">
+        <f>G40*$B$10</f>
+        <v>-1.0231815394945442E-13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="E41">
+        <f t="shared" si="4"/>
+        <v>244.99999999999994</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>596</v>
+      </c>
+      <c r="G41" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.1368683772161603E-13</v>
+      </c>
+      <c r="H41">
+        <f>G41*$B$10</f>
+        <v>-3.4106051316484808E-14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="2"/>
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="2"/>
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="2"/>
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="2"/>
+      <c r="B49" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
75. Multiple Terms in Action
</commit_message>
<xml_diff>
--- a/resources/mse_graph.xlsx
+++ b/resources/mse_graph.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noah/Documents/study/study_codes/udemy/machine-learning-js-stephen/machine-learning-js-stephen-git/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB53765A-0CBE-FA47-ACCD-286ED7B01F01}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C2B522-3059-A04E-A1BA-73C48BB5D7F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1680" yWindow="-20940" windowWidth="29980" windowHeight="18940" activeTab="1" xr2:uid="{4090F69A-B87C-A848-B205-CF8351D4CAAD}"/>
+    <workbookView xWindow="-5480" yWindow="-20560" windowWidth="29980" windowHeight="18940" activeTab="2" xr2:uid="{4090F69A-B87C-A848-B205-CF8351D4CAAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Gradient Descent" sheetId="3" r:id="rId2"/>
+    <sheet name="M + B" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Guess for B</t>
   </si>
@@ -63,6 +64,21 @@
   <si>
     <t>learning rate</t>
   </si>
+  <si>
+    <t>Slope of MSE WRT M</t>
+  </si>
+  <si>
+    <t>Slope of MSE WRT B</t>
+  </si>
+  <si>
+    <t>Value of M</t>
+  </si>
+  <si>
+    <t>Lot Size(Before Standardization)</t>
+  </si>
+  <si>
+    <t>Lot Size(standardized)</t>
+  </si>
 </sst>
 </file>
 
@@ -71,7 +87,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -86,6 +102,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -114,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -130,6 +152,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3749,7 +3773,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="3">
-        <f t="shared" ref="B10:B49" si="0">(($A11-$B$2)^2+($A11-$B$3)^2+($A11-$B$4)^2+($A11-$B$5)^2+($A11-$B$6)^2+($A11-$B$7)^2) / 6</f>
+        <f t="shared" ref="B11:B49" si="0">(($A11-$B$2)^2+($A11-$B$3)^2+($A11-$B$4)^2+($A11-$B$5)^2+($A11-$B$6)^2+($A11-$B$7)^2) / 6</f>
         <v>55352</v>
       </c>
     </row>
@@ -4143,8 +4167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1F2E40-F65D-B748-9EBC-90B3D8E3A982}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4198,7 +4222,7 @@
         <v>-490</v>
       </c>
       <c r="H2">
-        <f>G2*$B$10</f>
+        <f t="shared" ref="H2:H41" si="0">G2*$B$10</f>
         <v>-147</v>
       </c>
     </row>
@@ -4214,7 +4238,7 @@
         <v>147</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F41" si="0">((E3-$B$2)^2+(E3-$B$3)^2+(E3-$B$4)^2+(E3-$B$5)^2+(E3-$B$6)^2+(E3-$B$7)^2) / 6</f>
+        <f t="shared" ref="F3:F41" si="1">((E3-$B$2)^2+(E3-$B$3)^2+(E3-$B$4)^2+(E3-$B$5)^2+(E3-$B$6)^2+(E3-$B$7)^2) / 6</f>
         <v>10200</v>
       </c>
       <c r="G3" s="5">
@@ -4222,7 +4246,7 @@
         <v>-196</v>
       </c>
       <c r="H3">
-        <f>G3*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-58.8</v>
       </c>
     </row>
@@ -4234,19 +4258,19 @@
         <v>245</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E27" si="1">E3-H3</f>
+        <f t="shared" ref="E4:E27" si="2">E3-H3</f>
         <v>205.8</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2132.6399999999994</v>
       </c>
       <c r="G4" s="5">
-        <f t="shared" ref="G4:G41" si="2">2 * ((E4-$B$2) + (E4-$B$3) + (E4-$B$4) + (E4-$B$5) + (E4-$B$6) + (E4-$B$7)) / 6</f>
+        <f t="shared" ref="G4:G41" si="3">2 * ((E4-$B$2) + (E4-$B$3) + (E4-$B$4) + (E4-$B$5) + (E4-$B$6) + (E4-$B$7)) / 6</f>
         <v>-78.399999999999977</v>
       </c>
       <c r="H4">
-        <f>G4*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-23.519999999999992</v>
       </c>
     </row>
@@ -4258,19 +4282,19 @@
         <v>274</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>229.32</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>841.86240000000032</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-31.360000000000014</v>
       </c>
       <c r="H5">
-        <f>G5*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-9.408000000000003</v>
       </c>
     </row>
@@ -4282,19 +4306,19 @@
         <v>259</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>238.72800000000001</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>635.33798399999989</v>
       </c>
       <c r="G6" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-12.543999999999983</v>
       </c>
       <c r="H6">
-        <f>G6*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-3.7631999999999945</v>
       </c>
     </row>
@@ -4306,37 +4330,37 @@
         <v>262</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>242.49119999999999</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>602.29407744000002</v>
       </c>
       <c r="G7" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-5.0176000000000158</v>
       </c>
       <c r="H7">
-        <f>G7*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-1.5052800000000046</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>243.99647999999999</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>597.00705239039996</v>
       </c>
       <c r="G8" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2.0070400000000177</v>
       </c>
       <c r="H8">
-        <f>G8*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-0.60211200000000531</v>
       </c>
     </row>
@@ -4344,19 +4368,19 @@
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="E9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.598592</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.16112838246397</v>
       </c>
       <c r="G9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.80281600000000708</v>
       </c>
       <c r="H9">
-        <f>G9*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-0.24084480000000211</v>
       </c>
     </row>
@@ -4368,19 +4392,19 @@
         <v>0.3</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.83943679999999</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.02578054119431</v>
       </c>
       <c r="G10" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.32112640000002557</v>
       </c>
       <c r="H10">
-        <f>G10*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-9.6337920000007668E-2</v>
       </c>
     </row>
@@ -4389,19 +4413,19 @@
         <v>0.1</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.93577471999998</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00412488659106</v>
       </c>
       <c r="G11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.12845056000003297</v>
       </c>
       <c r="H11">
-        <f>G11*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-3.853516800000989E-2</v>
       </c>
     </row>
@@ -4410,19 +4434,19 @@
         <v>0.3</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.97430988799999</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00065998185448</v>
       </c>
       <c r="G12" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-5.1380224000013186E-2</v>
       </c>
       <c r="H12">
-        <f>G12*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-1.5414067200003954E-2</v>
       </c>
     </row>
@@ -4434,19 +4458,19 @@
         <v>0.9</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.98972395519999</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00010559709665</v>
       </c>
       <c r="G13" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2.0552089600016643E-2</v>
       </c>
       <c r="H13">
-        <f>G13*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-6.1656268800049929E-3</v>
       </c>
     </row>
@@ -4458,19 +4482,19 @@
         <v>0.98</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.99588958208</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00001689553551</v>
       </c>
       <c r="G14" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-8.2208358400066572E-3</v>
       </c>
       <c r="H14">
-        <f>G14*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-2.4662507520019973E-3</v>
       </c>
     </row>
@@ -4482,38 +4506,38 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.998355832832</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00000270328553</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.2883343359912942E-3</v>
       </c>
       <c r="H15">
-        <f>G15*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-9.8650030079738826E-4</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="E16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.9993423331328</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00000043252578</v>
       </c>
       <c r="G16" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1.3153337343965177E-3</v>
       </c>
       <c r="H16">
-        <f>G16*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-3.9460012031895532E-4</v>
       </c>
     </row>
@@ -4521,19 +4545,19 @@
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="E17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.99973693325313</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00000006920413</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-5.2613349373586971E-4</v>
       </c>
       <c r="H17">
-        <f>G17*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-1.578400481207609E-4</v>
       </c>
     </row>
@@ -4541,19 +4565,19 @@
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="E18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.99989477330126</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00000001107264</v>
       </c>
       <c r="G18" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2.1045339747161051E-4</v>
       </c>
       <c r="H18">
-        <f>G18*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-6.3136019241483149E-5</v>
       </c>
     </row>
@@ -4561,19 +4585,19 @@
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="E19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.9999579093205</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.0000000017717</v>
       </c>
       <c r="G19" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-8.418135900001289E-5</v>
       </c>
       <c r="H19">
-        <f>G19*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-2.5254407700003866E-5</v>
       </c>
     </row>
@@ -4581,19 +4605,19 @@
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="E20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.99998316372819</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00000000028342</v>
       </c>
       <c r="G20" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.3672543622742523E-5</v>
       </c>
       <c r="H20">
-        <f>G20*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-1.0101763086822757E-5</v>
       </c>
     </row>
@@ -4601,19 +4625,19 @@
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="E21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.99999326549127</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00000000004536</v>
       </c>
       <c r="G21" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1.3469017460465693E-5</v>
       </c>
       <c r="H21">
-        <f>G21*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-4.0407052381397078E-6</v>
       </c>
     </row>
@@ -4621,19 +4645,19 @@
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="E22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.99999730619652</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00000000000728</v>
       </c>
       <c r="G22" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-5.3876069614489097E-6</v>
       </c>
       <c r="H22">
-        <f>G22*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-1.6162820884346729E-6</v>
       </c>
     </row>
@@ -4641,19 +4665,19 @@
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="E23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.9999989224786</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00000000000125</v>
       </c>
       <c r="G23" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2.1550428073169314E-6</v>
       </c>
       <c r="H23">
-        <f>G23*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-6.4651284219507939E-7</v>
       </c>
     </row>
@@ -4661,19 +4685,19 @@
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="E24" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.99999956899143</v>
       </c>
       <c r="F24" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00000000000011</v>
       </c>
       <c r="G24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-8.6201714566414012E-7</v>
       </c>
       <c r="H24" s="8">
-        <f>G24*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-2.5860514369924202E-7</v>
       </c>
     </row>
@@ -4681,19 +4705,19 @@
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="E25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.99999982759658</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596</v>
       </c>
       <c r="G25" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.448068355282885E-7</v>
       </c>
       <c r="H25">
-        <f>G25*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-1.0344205065848655E-7</v>
       </c>
     </row>
@@ -4701,19 +4725,19 @@
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="E26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.99999993103864</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>595.99999999999989</v>
       </c>
       <c r="G26" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1.3792271147394786E-7</v>
       </c>
       <c r="H26">
-        <f>G26*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-4.1376813442184356E-8</v>
       </c>
     </row>
@@ -4721,19 +4745,19 @@
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="E27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.99999997241545</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00000000000011</v>
       </c>
       <c r="G27" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-5.5169095958262915E-8</v>
       </c>
       <c r="H27">
-        <f>G27*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-1.6550728787478874E-8</v>
       </c>
     </row>
@@ -4745,7 +4769,7 @@
         <v>244.99999998896618</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>595.99999999999989</v>
       </c>
       <c r="G28" s="5">
@@ -4753,7 +4777,7 @@
         <v>-2.2067638383305166E-8</v>
       </c>
       <c r="H28">
-        <f>G28*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-6.6202915149915494E-9</v>
       </c>
     </row>
@@ -4761,19 +4785,19 @@
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="E29">
-        <f t="shared" ref="E29:E33" si="3">E28-H28</f>
+        <f t="shared" ref="E29:E33" si="4">E28-H28</f>
         <v>244.99999999558648</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>595.99999999999989</v>
       </c>
       <c r="G29" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-8.8270439846382942E-9</v>
       </c>
       <c r="H29">
-        <f>G29*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-2.6481131953914882E-9</v>
       </c>
     </row>
@@ -4781,19 +4805,19 @@
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="E30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>244.99999999823459</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>595.99999999999989</v>
       </c>
       <c r="G30" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.5308289625390898E-9</v>
       </c>
       <c r="H30">
-        <f>G30*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-1.059248688761727E-9</v>
       </c>
     </row>
@@ -4801,19 +4825,19 @@
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="E31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>244.99999999929383</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596</v>
       </c>
       <c r="G31" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1.4123315850156359E-9</v>
       </c>
       <c r="H31">
-        <f>G31*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-4.2369947550469074E-10</v>
       </c>
     </row>
@@ -4821,19 +4845,19 @@
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="E32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>244.99999999971755</v>
       </c>
       <c r="F32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596</v>
       </c>
       <c r="G32" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-5.6490989663871005E-10</v>
       </c>
       <c r="H32">
-        <f>G32*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-1.6947296899161302E-10</v>
       </c>
     </row>
@@ -4841,19 +4865,19 @@
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="E33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>244.99999999988702</v>
       </c>
       <c r="F33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>595.99999999999989</v>
       </c>
       <c r="G33" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2.2595258997171186E-10</v>
       </c>
       <c r="H33">
-        <f>G33*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-6.7785776991513558E-11</v>
       </c>
     </row>
@@ -4865,7 +4889,7 @@
         <v>244.99999999995481</v>
       </c>
       <c r="F34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00000000000011</v>
       </c>
       <c r="G34" s="5">
@@ -4873,7 +4897,7 @@
         <v>-9.0381035988684744E-11</v>
       </c>
       <c r="H34">
-        <f>G34*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-2.7114310796605423E-11</v>
       </c>
     </row>
@@ -4881,19 +4905,19 @@
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="E35">
-        <f t="shared" ref="E35:E41" si="4">E34-H34</f>
+        <f t="shared" ref="E35:E41" si="5">E34-H34</f>
         <v>244.99999999998192</v>
       </c>
       <c r="F35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596</v>
       </c>
       <c r="G35" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.6152414395473897E-11</v>
       </c>
       <c r="H35">
-        <f>G35*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-1.0845724318642168E-11</v>
       </c>
     </row>
@@ -4901,19 +4925,19 @@
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
       <c r="E36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>244.99999999999278</v>
       </c>
       <c r="F36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596</v>
       </c>
       <c r="G36" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1.4438228390645236E-11</v>
       </c>
       <c r="H36">
-        <f>G36*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-4.3314685171935709E-12</v>
       </c>
     </row>
@@ -4921,19 +4945,19 @@
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="E37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>244.9999999999971</v>
       </c>
       <c r="F37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00000000000011</v>
       </c>
       <c r="G37" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-5.7980287238024175E-12</v>
       </c>
       <c r="H37">
-        <f>G37*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-1.7394086171407251E-12</v>
       </c>
     </row>
@@ -4941,19 +4965,19 @@
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="E38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>244.99999999999883</v>
       </c>
       <c r="F38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00000000000011</v>
       </c>
       <c r="G38" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2.3305801732931286E-12</v>
       </c>
       <c r="H38">
-        <f>G38*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-6.9917405198793852E-13</v>
       </c>
     </row>
@@ -4961,19 +4985,19 @@
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="E39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>244.99999999999955</v>
       </c>
       <c r="F39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596</v>
       </c>
       <c r="G39" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-9.0949470177292824E-13</v>
       </c>
       <c r="H39">
-        <f>G39*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-2.7284841053187846E-13</v>
       </c>
     </row>
@@ -4981,19 +5005,19 @@
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="E40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>244.99999999999983</v>
       </c>
       <c r="F40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.00000000000011</v>
       </c>
       <c r="G40" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.4106051316484809E-13</v>
       </c>
       <c r="H40">
-        <f>G40*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-1.0231815394945442E-13</v>
       </c>
     </row>
@@ -5001,19 +5025,19 @@
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="E41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>244.99999999999994</v>
       </c>
       <c r="F41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596</v>
       </c>
       <c r="G41" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1.1368683772161603E-13</v>
       </c>
       <c r="H41">
-        <f>G41*$B$10</f>
+        <f t="shared" si="0"/>
         <v>-3.4106051316484808E-14</v>
       </c>
     </row>
@@ -5053,4 +5077,1256 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{507B816E-4DD8-5F47-8BBC-B45A9CABF945}">
+  <dimension ref="A1:I49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="12.83203125" customWidth="1"/>
+    <col min="4" max="5" width="12.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="12">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>200</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <f>(2/6) * ((-$A$2*($B$2 - (D2*$A$2 +E2))) + (-$A$3*($B$3 - (D2*$A$3 +E2))) + (-$A$4*($B$4 - (D2*$A$4 +E2))) + (-$A$5*($B$5 - (D2*$A$5 +E2))) + (-$A$6*($B$6 - (D2*$A$6 +E2))) + (-$A$7*($B$7 - (D2*$A$7 +E2))))</f>
+        <v>-275.76666666666665</v>
+      </c>
+      <c r="G2" s="5">
+        <f>(2/6) * ((-1 *($B$2-(D2*$A$2 + E2)))+ (-1 *($B$3-(D2*$A$3 + E2)))+ (-1 *($B$4-(D2*$A$4 + E2)))+ (-1 *($B$5-(D2*$A$5 + E2)))+ (-1 *($B$6-(D2*$A$6 + E2)))+ (-1 *($B$7-(D2*$A$7 + E2))))</f>
+        <v>-490</v>
+      </c>
+      <c r="H2">
+        <f>F2*$B$10</f>
+        <v>-179.24833333333333</v>
+      </c>
+      <c r="I2">
+        <f>G2*$B$10</f>
+        <v>-318.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="B3" s="1">
+        <v>230</v>
+      </c>
+      <c r="D3" s="2">
+        <f>D2-H2</f>
+        <v>179.24833333333333</v>
+      </c>
+      <c r="E3" s="2">
+        <f>E2-I2</f>
+        <v>318.5</v>
+      </c>
+      <c r="F3" s="5">
+        <f>(2/6) * ((-$A$2*($B$2 - (D3*$A$2 +E3))) + (-$A$3*($B$3 - (D3*$A$3 +E3))) + (-$A$4*($B$4 - (D3*$A$4 +E3))) + (-$A$5*($B$5 - (D3*$A$5 +E3))) + (-$A$6*($B$6 - (D3*$A$6 +E3))) + (-$A$7*($B$7 - (D3*$A$7 +E3))))</f>
+        <v>205.87159722222225</v>
+      </c>
+      <c r="G3" s="5">
+        <f>(2/6) * ((-1 *($B$2-(D3*$A$2 + E3)))+ (-1 *($B$3-(D3*$A$3 + E3)))+ (-1 *($B$4-(D3*$A$4 + E3)))+ (-1 *($B$5-(D3*$A$5 + E3)))+ (-1 *($B$6-(D3*$A$6 + E3)))+ (-1 *($B$7-(D3*$A$7 + E3))))</f>
+        <v>338.19822222222223</v>
+      </c>
+      <c r="H3">
+        <f>F3*$B$10</f>
+        <v>133.81653819444446</v>
+      </c>
+      <c r="I3">
+        <f>G3*$B$10</f>
+        <v>219.82884444444446</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>245</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D41" si="0">D3-H3</f>
+        <v>45.431795138888873</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" ref="E4:E41" si="1">E3-I3</f>
+        <v>98.671155555555544</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" ref="F4:F41" si="2">(2/6) * ((-$A$2*($B$2 - (D4*$A$2 +E4))) + (-$A$3*($B$3 - (D4*$A$3 +E4))) + (-$A$4*($B$4 - (D4*$A$4 +E4))) + (-$A$5*($B$5 - (D4*$A$5 +E4))) + (-$A$6*($B$6 - (D4*$A$6 +E4))) + (-$A$7*($B$7 - (D4*$A$7 +E4))))</f>
+        <v>-134.55059625578704</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" ref="G4:G41" si="3">(2/6) * ((-1 *($B$2-(D4*$A$2 + E4)))+ (-1 *($B$3-(D4*$A$3 + E4)))+ (-1 *($B$4-(D4*$A$4 + E4)))+ (-1 *($B$5-(D4*$A$5 + E4)))+ (-1 *($B$6-(D4*$A$6 + E4)))+ (-1 *($B$7-(D4*$A$7 + E4))))</f>
+        <v>-244.19710740740746</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H41" si="4">F4*$B$10</f>
+        <v>-87.457887566261576</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I41" si="5">G4*$B$10</f>
+        <v>-158.72811981481485</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="B5" s="1">
+        <v>274</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>132.88968270515045</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="1"/>
+        <v>257.39927537037039</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" si="2"/>
+        <v>103.99689253663919</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" si="3"/>
+        <v>166.54754562623461</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="4"/>
+        <v>67.597980148815481</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="5"/>
+        <v>108.2559046570525</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>259</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>65.291702556334968</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>149.14337071331789</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" si="2"/>
+        <v>-64.991140048695726</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="3"/>
+        <v>-122.06877584660693</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="4"/>
+        <v>-42.244241031652223</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="5"/>
+        <v>-79.344704300294509</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="12">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>262</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>107.53594358798719</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>228.48807501361239</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="2"/>
+        <v>53.086568688343064</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="3"/>
+        <v>81.681156521077781</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="4"/>
+        <v>34.50626964742299</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="5"/>
+        <v>53.092751738700557</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>73.029673940564209</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>175.39532327491185</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="2"/>
+        <v>-30.863163303814037</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="3"/>
+        <v>-61.311034580241156</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>-20.061056147479125</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="5"/>
+        <v>-39.852172477156749</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>93.09073008804333</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>215.2474957520686</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="2"/>
+        <v>27.527490121907494</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="3"/>
+        <v>39.791770264716774</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="4"/>
+        <v>17.89286857923987</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="5"/>
+        <v>25.864650672065903</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0.65</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>75.197861508803456</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>189.38284508000271</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" si="2"/>
+        <v>-14.226658220194375</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="3"/>
+        <v>-31.023257563937563</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="4"/>
+        <v>-9.2473278431263441</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="5"/>
+        <v>-20.165117416559415</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>84.445189351929798</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>209.54796249656212</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" si="2"/>
+        <v>14.603601566610687</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" si="3"/>
+        <v>19.17079363518269</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="4"/>
+        <v>9.4923410182969459</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="5"/>
+        <v>12.461015862868749</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>0.1</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>74.952848333632858</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>197.08694663369337</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="2"/>
+        <v>-6.2029186599343875</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="3"/>
+        <v>-15.876401843404864</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="4"/>
+        <v>-4.0318971289573522</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="5"/>
+        <v>-10.319661198213161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>0.3</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>78.984745462590212</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>207.40660783190654</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="2"/>
+        <v>7.9966385119175616</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="3"/>
+        <v>9.0636108239093094</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="4"/>
+        <v>5.1978150327464148</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="5"/>
+        <v>5.8913470355410515</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>0.9</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>73.786930429843792</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>201.51526079636548</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.4024018935838178</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" si="3"/>
+        <v>-8.263419282102328</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="4"/>
+        <v>-1.5615612308294817</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="5"/>
+        <v>-5.3712225333665131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>0.98</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>75.348491660673275</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>206.88648332973199</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="2"/>
+        <v>4.5631381164137927</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" si="3"/>
+        <v>4.1446910975154667</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
+        <v>2.9660397756689654</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="5"/>
+        <v>2.6940492133850533</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>72.382451885004315</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>204.19243411634693</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="2"/>
+        <v>-0.65862920026818605</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.4071830899681945</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>-0.42810898017432097</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="5"/>
+        <v>-2.8646690084793267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>72.81056086517863</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>207.05710312482626</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="shared" si="2"/>
+        <v>2.7359373514144161</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="3"/>
+        <v>1.7788045058430459</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="4"/>
+        <v>1.7783592784193705</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="5"/>
+        <v>1.1562229287979799</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>71.032201586759257</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>205.90088019602828</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" si="2"/>
+        <v>9.4765131947918718E-2</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" si="3"/>
+        <v>-2.4305579154002239</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="4"/>
+        <v>6.159733576614717E-2</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="5"/>
+        <v>-1.5798626450101456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>70.970604250993105</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="1"/>
+        <v>207.48074284103842</v>
+      </c>
+      <c r="F19" s="5">
+        <f t="shared" si="2"/>
+        <v>1.7311873958105217</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="3"/>
+        <v>0.66346354980281785</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="4"/>
+        <v>1.1252718072768391</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="5"/>
+        <v>0.43125130737183159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>800</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>69.845332443716259</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
+        <v>207.04949153366658</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" si="2"/>
+        <v>0.38034582051972343</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.3993289927028247</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="4"/>
+        <v>0.24722478333782025</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="5"/>
+        <v>-0.90956384525683609</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>950</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>69.598107660378446</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="1"/>
+        <v>207.95905537892341</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" si="2"/>
+        <v>1.1548276353178981</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="3"/>
+        <v>0.15609226225048661</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="4"/>
+        <v>0.75063796295663376</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="5"/>
+        <v>0.1014599704628163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>1040</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>68.847469697421815</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="1"/>
+        <v>207.85759540846058</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" si="2"/>
+        <v>0.45234861281689831</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.84750817249555621</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="4"/>
+        <v>0.29402659833098393</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="5"/>
+        <v>-0.55088031212211153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>1120</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>68.553443099090828</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="1"/>
+        <v>208.40847572058269</v>
+      </c>
+      <c r="F23" s="5">
+        <f t="shared" si="2"/>
+        <v>0.80718322206844739</v>
+      </c>
+      <c r="G23" s="5">
+        <f t="shared" si="3"/>
+        <v>-5.9375919804400226E-2</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="4"/>
+        <v>0.52466909434449083</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="5"/>
+        <v>-3.8594347872860146E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>1250</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>68.028774004746339</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="1"/>
+        <v>208.44707006845556</v>
+      </c>
+      <c r="F24" s="5">
+        <f t="shared" si="2"/>
+        <v>0.43298749344343845</v>
+      </c>
+      <c r="G24" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.54183425802613283</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="4"/>
+        <v>0.28144187073823501</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="5"/>
+        <v>-0.35219226771698636</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>1350</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>67.747332134008104</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="1"/>
+        <v>208.79926233617255</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" si="2"/>
+        <v>0.5858510980071252</v>
+      </c>
+      <c r="G25" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.1376543847129407</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="4"/>
+        <v>0.38080321370463138</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="5"/>
+        <v>-8.9475350063411452E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>67.366528920303466</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="1"/>
+        <v>208.88873768623597</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" si="2"/>
+        <v>0.37982226055860835</v>
+      </c>
+      <c r="G26" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.36489377920436061</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="4"/>
+        <v>0.24688446936309544</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="5"/>
+        <v>-0.23718095648283441</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>67.11964445094037</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="1"/>
+        <v>209.1259186427188</v>
+      </c>
+      <c r="F27" s="5">
+        <f t="shared" si="2"/>
+        <v>0.43736507589450407</v>
+      </c>
+      <c r="G27" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.15387530022600987</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="4"/>
+        <v>0.28428729933142766</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="5"/>
+        <v>-0.10001894514690642</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>66.835357151608946</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="1"/>
+        <v>209.2259375878657</v>
+      </c>
+      <c r="F28" s="5">
+        <f t="shared" si="2"/>
+        <v>0.31899117208049194</v>
+      </c>
+      <c r="G28" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.25707719588572786</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="4"/>
+        <v>0.20734426185231977</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="5"/>
+        <v>-0.1671001773257231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>66.628012889756633</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="1"/>
+        <v>209.39303776519142</v>
+      </c>
+      <c r="F29" s="5">
+        <f t="shared" si="2"/>
+        <v>0.33308382059485631</v>
+      </c>
+      <c r="G29" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.14404405387674046</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="4"/>
+        <v>0.21650448338665659</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="5"/>
+        <v>-9.3628635019881307E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>66.411508406369975</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="1"/>
+        <v>209.48666640021131</v>
+      </c>
+      <c r="F30" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26155498193495674</v>
+      </c>
+      <c r="G30" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.18772489944941145</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="4"/>
+        <v>0.17001073825772189</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="5"/>
+        <v>-0.12202118464211745</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>66.24149766811226</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="1"/>
+        <v>209.60868758485341</v>
+      </c>
+      <c r="F31" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2571190777658412</v>
+      </c>
+      <c r="G31" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.12502731764010377</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="4"/>
+        <v>0.16712740054779679</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="5"/>
+        <v>-8.1267756466067459E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>66.074370267564461</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="1"/>
+        <v>209.68995534131949</v>
+      </c>
+      <c r="F32" s="5">
+        <f t="shared" si="2"/>
+        <v>0.21149549256266492</v>
+      </c>
+      <c r="G32" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.14076103195891201</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="4"/>
+        <v>0.13747207016573221</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="5"/>
+        <v>-9.1494670773292819E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="D33" s="2">
+        <f t="shared" si="0"/>
+        <v>65.936898197398733</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="1"/>
+        <v>209.78145001209279</v>
+      </c>
+      <c r="F33" s="5">
+        <f t="shared" si="2"/>
+        <v>0.20025775250631028</v>
+      </c>
+      <c r="G33" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.10440856525576692</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="4"/>
+        <v>0.1301675391291017</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="5"/>
+        <v>-6.7865567416248496E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>65.806730658269629</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="1"/>
+        <v>209.84931557950904</v>
+      </c>
+      <c r="F34" s="5">
+        <f t="shared" si="2"/>
+        <v>0.16959838927311566</v>
+      </c>
+      <c r="G34" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.10752280549429352</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="4"/>
+        <v>0.11023895302752518</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="5"/>
+        <v>-6.9889823571290796E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>65.69649170524211</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="1"/>
+        <v>209.91920540308033</v>
+      </c>
+      <c r="F35" s="5">
+        <f t="shared" si="2"/>
+        <v>0.15687502993568181</v>
+      </c>
+      <c r="G35" s="5">
+        <f t="shared" si="3"/>
+        <v>-8.533137491443199E-2</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="4"/>
+        <v>0.10196876945819318</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="5"/>
+        <v>-5.5465393694380798E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>65.594522935783914</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="1"/>
+        <v>209.97467079677472</v>
+      </c>
+      <c r="F36" s="5">
+        <f t="shared" si="2"/>
+        <v>0.13531284072195918</v>
+      </c>
+      <c r="G36" s="5">
+        <f t="shared" si="3"/>
+        <v>-8.3167274947726355E-2</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="4"/>
+        <v>8.7953346469273469E-2</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="5"/>
+        <v>-5.4058728716022131E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="3"/>
+      <c r="D37" s="2">
+        <f t="shared" si="0"/>
+        <v>65.506569589314637</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="1"/>
+        <v>210.02872952549075</v>
+      </c>
+      <c r="F37" s="5">
+        <f t="shared" si="2"/>
+        <v>0.12334575206421761</v>
+      </c>
+      <c r="G37" s="5">
+        <f t="shared" si="3"/>
+        <v>-6.886672041623379E-2</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="4"/>
+        <v>8.017473884174145E-2</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="5"/>
+        <v>-4.4763368270551968E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="3"/>
+      <c r="D38" s="2">
+        <f t="shared" si="0"/>
+        <v>65.426394850472889</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="1"/>
+        <v>210.07349289376131</v>
+      </c>
+      <c r="F38" s="5">
+        <f t="shared" si="2"/>
+        <v>0.1076216766364535</v>
+      </c>
+      <c r="G38" s="5">
+        <f t="shared" si="3"/>
+        <v>-6.4859705306275828E-2</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="4"/>
+        <v>6.9954089813694775E-2</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="5"/>
+        <v>-4.2158808449079287E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="D39" s="2">
+        <f t="shared" si="0"/>
+        <v>65.356440760659197</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="1"/>
+        <v>210.11565170221039</v>
+      </c>
+      <c r="F39" s="5">
+        <f t="shared" si="2"/>
+        <v>9.7210751212936458E-2</v>
+      </c>
+      <c r="G39" s="5">
+        <f t="shared" si="3"/>
+        <v>-5.5159784209422469E-2</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="4"/>
+        <v>6.3186988288408699E-2</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="5"/>
+        <v>-3.5853859736124608E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="3"/>
+      <c r="D40" s="2">
+        <f t="shared" si="0"/>
+        <v>65.29325377237079</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="1"/>
+        <v>210.15150556194652</v>
+      </c>
+      <c r="F40" s="5">
+        <f t="shared" si="2"/>
+        <v>8.5431835869838338E-2</v>
+      </c>
+      <c r="G40" s="5">
+        <f t="shared" si="3"/>
+        <v>-5.085151891143861E-2</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="4"/>
+        <v>5.5530693315394924E-2</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="5"/>
+        <v>-3.3053487292435096E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="D41" s="2">
+        <f t="shared" si="0"/>
+        <v>65.237723079055399</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="1"/>
+        <v>210.18455904923897</v>
+      </c>
+      <c r="F41" s="5">
+        <f t="shared" si="2"/>
+        <v>7.6727090107086809E-2</v>
+      </c>
+      <c r="G41" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.3977283862972172E-2</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="4"/>
+        <v>4.987260856960643E-2</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="5"/>
+        <v>-2.8585234510931912E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="2"/>
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="2"/>
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="2"/>
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="2"/>
+      <c r="B49" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>